<commit_message>
with comments from meeting with Alex
</commit_message>
<xml_diff>
--- a/documents/Heat Estimation.xlsx
+++ b/documents/Heat Estimation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam Welser\Documents\Studium\Master\Vorlesungen\3. Semester\Praktikum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{969C5073-58D3-4DEC-A49E-C3695A3E6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B061DBE3-DD59-408B-8AFC-05C137470879}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="-120" windowWidth="28110" windowHeight="18240" xr2:uid="{677E9D87-799D-4A99-A7DE-60C845394385}"/>
+    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="18240" xr2:uid="{677E9D87-799D-4A99-A7DE-60C845394385}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="9V -&gt; 5V" sheetId="1" r:id="rId1"/>
+    <sheet name="5V -&gt; 3.3V" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="76">
   <si>
     <t>Heat estimation for voltage regulator</t>
   </si>
@@ -153,17 +154,122 @@
     <t>Voltage Regulator without Heat Sink</t>
   </si>
   <si>
-    <t>Voltage Regulator with Heat Sink</t>
-  </si>
-  <si>
     <t>e.g. for parts that are not included in the calculation</t>
+  </si>
+  <si>
+    <t>Note: internally consumed current is neglected because load current is much higher</t>
+  </si>
+  <si>
+    <t>Voltage Regulator with PCB as Heat Sink</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>mm²</t>
+  </si>
+  <si>
+    <t>RthPCB</t>
+  </si>
+  <si>
+    <t>bei 100 cm²</t>
+  </si>
+  <si>
+    <t>We need an external heat sink!!!</t>
+  </si>
+  <si>
+    <t>Thermal Resistance of PCB</t>
+  </si>
+  <si>
+    <t>Voltage Regulator with External Heat Sink</t>
+  </si>
+  <si>
+    <t>RthThermalCompound</t>
+  </si>
+  <si>
+    <t>[W/mK]</t>
+  </si>
+  <si>
+    <t>m²</t>
+  </si>
+  <si>
+    <t>Thermal conductivity Compound</t>
+  </si>
+  <si>
+    <t>Area of voltage regulator</t>
+  </si>
+  <si>
+    <t>thickness of Compound</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Heat Sink</t>
+  </si>
+  <si>
+    <t>Fischer Elektronik Kühlkörper 6K/W, 32mm x 20mm x 50mm, Schraubmontage</t>
+  </si>
+  <si>
+    <t>AAVID THERMALLOY Kühlkörper 8.8K/W, 50mm x 34.5mm x 50mm, Lötmontage</t>
+  </si>
+  <si>
+    <t>Heat Sink 2</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/kuhlkorper/2212182</t>
+  </si>
+  <si>
+    <t>https://de.rs-online.com/web/p/kuhlkorper/0403184</t>
+  </si>
+  <si>
+    <t>RthHeatSink1</t>
+  </si>
+  <si>
+    <t>RthHeatSink2</t>
+  </si>
+  <si>
+    <t>Estimated junction temp. TJ1</t>
+  </si>
+  <si>
+    <t>Estimated junction temp. TJ2</t>
+  </si>
+  <si>
+    <t>Both external heat sinks can be used because the temperature remains &lt; 125°C</t>
+  </si>
+  <si>
+    <t>-&gt; needs at least +2V as input</t>
+  </si>
+  <si>
+    <t>-&gt; needs at least +1.5V as input</t>
+  </si>
+  <si>
+    <t>LM1085 IT-3.3</t>
+  </si>
+  <si>
+    <t>We do not need a heat sink</t>
+  </si>
+  <si>
+    <t>maximum value -&gt; low current LED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +289,22 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -209,13 +331,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -272,6 +398,423 @@
         <a:xfrm>
           <a:off x="5781675" y="3600450"/>
           <a:ext cx="3267075" cy="1197927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4000147</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>67254</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FBEA1B87-8F12-4ED9-A052-0D16DFE24CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5905501" y="6019799"/>
+          <a:ext cx="3485796" cy="1857955"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4400550</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Grafik 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09BDB544-58E4-4360-8750-28B8B7F2497A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="9791700" y="5467350"/>
+          <a:ext cx="5762625" cy="3238500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Textfeld 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13F658AF-15E4-4161-83DB-853AC776ECC6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="14487525" y="7305675"/>
+          <a:ext cx="1009650" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>1 oz</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t> copper</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>--&gt;</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100" baseline="0"/>
+            <a:t>0.0035 cm thickness</a:t>
+          </a:r>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>2553006</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9983B49F-0943-4225-8146-5735DB6F3330}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6067425" y="8696325"/>
+          <a:ext cx="2191056" cy="647790"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>74781</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3743325</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>77145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Grafik 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7619CEF2-5CE9-42DD-B221-FC56EBFBD1B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6381750" y="11552406"/>
+          <a:ext cx="3067050" cy="3812364"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4552950</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>181186</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>224402</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Grafik 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C2291420-B1B7-4A71-B466-3DA384875B09}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10258425" y="11468311"/>
+          <a:ext cx="4539227" cy="3209713"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3657600</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>35877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{412ED42A-31B0-4A5B-B626-F3670028BA97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6096000" y="3648075"/>
+          <a:ext cx="3267075" cy="1197927"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>619606</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171943</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Grafik 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{759C9B0B-3D96-4F9C-84F9-74DA5327A58C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12506325" y="1257300"/>
+          <a:ext cx="3448531" cy="3534268"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -580,23 +1123,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{102A874D-2BD9-4C2F-A65E-ED7E650AF54A}">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="70.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
@@ -630,17 +1174,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E6" s="2">
         <f>C6*D6</f>
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>2</v>
@@ -672,14 +1216,14 @@
         <v>9</v>
       </c>
       <c r="C8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
         <v>60</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
@@ -761,7 +1305,7 @@
       <c r="D13" s="2"/>
       <c r="E13" s="2">
         <f>SUM(E6:E11)</f>
-        <v>569</v>
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -769,15 +1313,15 @@
         <v>18</v>
       </c>
       <c r="C14" s="2">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2">
         <f>E13*C14</f>
-        <v>853.5</v>
+        <v>514.79999999999995</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
@@ -791,6 +1335,11 @@
         <v>22</v>
       </c>
     </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>24</v>
@@ -864,10 +1413,13 @@
       </c>
       <c r="C27">
         <f>(C25-C26)*E14/1000</f>
-        <v>3.4140000000000001</v>
+        <v>2.0591999999999997</v>
       </c>
       <c r="D27" t="s">
         <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
@@ -876,23 +1428,23 @@
       </c>
       <c r="C28">
         <f>C22+C20*C27</f>
-        <v>192.70000000000002</v>
+        <v>124.95999999999998</v>
       </c>
       <c r="D28" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>25</v>
       </c>
@@ -901,6 +1453,236 @@
       </c>
       <c r="D35" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36">
+        <v>35</v>
+      </c>
+      <c r="D36" t="s">
+        <v>27</v>
+      </c>
+      <c r="E36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37">
+        <f>C46/(C45*C47)</f>
+        <v>8.7108298394227166</v>
+      </c>
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <f>C22+(C35+C36+C37)*C27</f>
+        <v>122.30534080533924</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>42</v>
+      </c>
+      <c r="C41">
+        <v>10</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42">
+        <v>15.25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43">
+        <v>3.85</v>
+      </c>
+      <c r="D43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44">
+        <f>C41*C42-C43^2*PI()/4</f>
+        <v>140.85843572304131</v>
+      </c>
+      <c r="D44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45">
+        <f>C44*10^-6</f>
+        <v>1.4085843572304131E-4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46">
+        <v>1E-3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D47" t="s">
+        <v>54</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54">
+        <v>5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <f>C46/(C45*C47)</f>
+        <v>8.7108298394227166</v>
+      </c>
+      <c r="D55" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>66</v>
+      </c>
+      <c r="C56">
+        <v>6</v>
+      </c>
+      <c r="D56" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>67</v>
+      </c>
+      <c r="C57">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="D57" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58">
+        <f>C22+(C54+C55+C56)*C27</f>
+        <v>62.58854080533925</v>
+      </c>
+      <c r="D58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59">
+        <f>C22+(C54+C55+C57)*C27</f>
+        <v>68.35430080533925</v>
+      </c>
+      <c r="D59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -911,6 +1693,344 @@
     <hyperlink ref="G9" r:id="rId4" xr:uid="{52F5BE9F-1E78-48FB-8E63-C325FEBA4A1E}"/>
     <hyperlink ref="G10" r:id="rId5" xr:uid="{EFD41A75-A25B-4E0E-98F4-F613651CCFC9}"/>
     <hyperlink ref="G18" r:id="rId6" xr:uid="{66E4EB7D-B73B-45F8-8FA0-62BB59D1A9E9}"/>
+    <hyperlink ref="G47" r:id="rId7" xr:uid="{4B7DB915-F261-40FD-A695-9CDC7B98C908}"/>
+    <hyperlink ref="G56" r:id="rId8" xr:uid="{9618B2B4-4357-4164-BECC-4595855D458B}"/>
+    <hyperlink ref="G57" r:id="rId9" xr:uid="{81118654-95A5-4799-A0A2-741C51E62424}"/>
+    <hyperlink ref="H56" r:id="rId10" xr:uid="{92E17419-DEBF-4AE4-BBCA-86B004E64BE5}"/>
+    <hyperlink ref="H57" r:id="rId11" xr:uid="{411C6EAE-4EE0-4389-9692-81D4E0E96691}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId12"/>
+  <drawing r:id="rId13"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF64E67B-8E08-45C2-A8F7-CE9D61538ED4}">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="32.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>30</v>
+      </c>
+      <c r="E6" s="2">
+        <f>C6*D6</f>
+        <v>150</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2">
+        <v>3</v>
+      </c>
+      <c r="D7" s="2">
+        <v>22</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" ref="E7:E11" si="0">C7*D7</f>
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
+        <v>120</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="2">
+        <v>250</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
+        <v>250</v>
+      </c>
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1</v>
+      </c>
+      <c r="D10" s="2">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>30</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <f>SUM(E6:E11)</f>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <f>E13*C14</f>
+        <v>943.5</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>125</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>22</v>
+      </c>
+      <c r="D22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23">
+        <f>(C21-C22)/C20</f>
+        <v>2.06</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26">
+        <v>3.3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27">
+        <f>(C25-C26)*E14/1000</f>
+        <v>1.6039500000000002</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28">
+        <f>C22+C20*C27</f>
+        <v>102.19750000000001</v>
+      </c>
+      <c r="D28" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G6" r:id="rId1" xr:uid="{F86ED6EF-C8CE-46AA-ACC7-96C19CB137F8}"/>
+    <hyperlink ref="G7" r:id="rId2" xr:uid="{12837959-56C8-469D-A9A7-D77D9C689E00}"/>
+    <hyperlink ref="G8" r:id="rId3" xr:uid="{99C9F20B-F986-4500-B759-A992C8354E1B}"/>
+    <hyperlink ref="G9" r:id="rId4" xr:uid="{5D03E3A9-1CFD-4C88-8437-3C3120EA6A54}"/>
+    <hyperlink ref="G10" r:id="rId5" xr:uid="{8E0A8201-F8CB-41D8-A7E2-37BAC825F02D}"/>
+    <hyperlink ref="G18" r:id="rId6" xr:uid="{5A3DC362-BF8C-4F14-A764-6EC09751A9D9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>

</xml_diff>